<commit_message>
Proposta Tecnica Financeira Actualizada
</commit_message>
<xml_diff>
--- a/ESWII/SAPDR_Plano_Negocio.xlsx
+++ b/ESWII/SAPDR_Plano_Negocio.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="82">
   <si>
     <t>Designacao do Especialista</t>
   </si>
@@ -316,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -325,31 +325,53 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -360,7 +382,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -370,9 +392,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -380,19 +403,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
@@ -883,14 +910,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="2:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -961,10 +988,10 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="13"/>
       <c r="D8">
         <f>SUM(Table1[Tempo em Hora])</f>
         <v>16</v>
@@ -987,14 +1014,14 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1101,10 +1128,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="13"/>
       <c r="D16">
         <f>SUM(Table14[Tempo em Hora])</f>
         <v>60</v>
@@ -1127,15 +1154,15 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -1245,10 +1272,10 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="10"/>
       <c r="D27">
         <f>SUM(Table145[Tempo em Hora])</f>
         <v>20</v>
@@ -1267,14 +1294,14 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -1367,10 +1394,10 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="13"/>
       <c r="D36">
         <f>SUM(Table1453[Tempo em Hora])</f>
         <v>25</v>
@@ -1389,14 +1416,14 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -1475,10 +1502,10 @@
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="12"/>
+      <c r="C45" s="13"/>
       <c r="D45">
         <f>SUM(Table14536[Tempo em Hora])</f>
         <v>20</v>
@@ -1498,16 +1525,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B19:H19"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B19:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1540,13 +1567,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="3" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -1763,7 +1790,7 @@
       <c r="C17">
         <v>14</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="4"/>
@@ -1774,7 +1801,7 @@
       <c r="C18">
         <v>15</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>59</v>
       </c>
       <c r="N18" s="3"/>
@@ -1783,7 +1810,7 @@
       <c r="C19">
         <v>16</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>60</v>
       </c>
       <c r="M19" s="4"/>
@@ -1794,7 +1821,7 @@
       <c r="C20">
         <v>17</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>61</v>
       </c>
       <c r="P20" s="3"/>
@@ -1803,7 +1830,7 @@
       <c r="C21">
         <v>18</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P21" s="3"/>
@@ -1813,7 +1840,7 @@
       <c r="C22">
         <v>19</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>63</v>
       </c>
       <c r="R22" s="3"/>
@@ -1822,7 +1849,7 @@
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>64</v>
       </c>
       <c r="R23" s="3"/>
@@ -1837,7 +1864,7 @@
       <c r="C24">
         <v>21</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>65</v>
       </c>
       <c r="T24" s="3"/>
@@ -1846,7 +1873,7 @@
       <c r="C25">
         <v>22</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>66</v>
       </c>
       <c r="T25" s="3"/>
@@ -1859,7 +1886,7 @@
       <c r="C26">
         <v>23</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>67</v>
       </c>
       <c r="V26" s="3"/>
@@ -1899,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:I57"/>
+  <dimension ref="C4:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,1068 +1942,1074 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="15" t="str">
+    <row r="5" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="14" t="str">
         <f>Sheet1!B3</f>
         <v>Grupo de processo de Inicialização</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="str">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="15" t="str">
         <f>Sheet1!B4</f>
         <v>Codigo</v>
       </c>
-      <c r="D6" s="7" t="str">
+      <c r="D6" s="15" t="str">
         <f>Sheet1!C4</f>
         <v>Designacao do Especialista</v>
       </c>
-      <c r="E6" s="7" t="str">
+      <c r="E6" s="15" t="str">
         <f>Sheet1!D4</f>
         <v>Tempo em Hora</v>
       </c>
-      <c r="F6" s="7" t="str">
+      <c r="F6" s="15" t="str">
         <f>Sheet1!E4</f>
         <v>Custo Por Hora</v>
       </c>
-      <c r="G6" s="7" t="str">
+      <c r="G6" s="15" t="str">
         <f>Sheet1!F4</f>
         <v>Quantidade</v>
       </c>
-      <c r="H6" s="7" t="str">
+      <c r="H6" s="15" t="str">
         <f>Sheet1!G4</f>
         <v>Custo Total</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="7">
+    <row r="7" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="15">
         <f>Sheet1!B5</f>
         <v>1</v>
       </c>
-      <c r="D7" s="7" t="str">
+      <c r="D7" s="15" t="str">
         <f>Sheet1!C5</f>
         <v>Analista do Sistema</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="15">
         <f>Sheet1!D5</f>
         <v>10</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="15">
         <f>Sheet1!E5</f>
         <v>300</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="15">
         <f>Sheet1!F5</f>
         <v>1</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="15">
         <f>Sheet1!G5</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="8" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="7">
+    <row r="8" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="15">
         <f>Sheet1!B6</f>
         <v>2</v>
       </c>
-      <c r="D8" s="7" t="str">
+      <c r="D8" s="15" t="str">
         <f>Sheet1!C6</f>
         <v>Gestor de Projecto</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="15">
         <f>Sheet1!D6</f>
         <v>6</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="15">
         <f>Sheet1!E6</f>
         <v>500</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="15">
         <f>Sheet1!F6</f>
         <v>1</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="15">
         <f>Sheet1!G6</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="str">
+    <row r="9" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="15" t="str">
         <f>Sheet1!B8</f>
         <v>Total</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D9" s="15">
         <f>Sheet1!C8</f>
         <v>0</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E9" s="15">
         <f>Sheet1!D8</f>
         <v>16</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F9" s="15">
         <f>Sheet1!E8</f>
         <v>800</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G9" s="15">
         <f>Sheet1!F8</f>
         <v>2</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H9" s="15">
         <f>Sheet1!G8</f>
         <v>6000</v>
       </c>
     </row>
-    <row r="11" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="16" t="str">
+    <row r="10" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="14" t="str">
         <f>Sheet1!B10</f>
         <v>Grupo de processo de Planejamento</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="8" t="str">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="15" t="str">
         <f>Sheet1!B11</f>
         <v>Codigo</v>
       </c>
-      <c r="D13" s="8" t="str">
+      <c r="D12" s="15" t="str">
         <f>Sheet1!C11</f>
         <v>Designacao do Especialista</v>
       </c>
-      <c r="E13" s="8" t="str">
+      <c r="E12" s="15" t="str">
         <f>Sheet1!D11</f>
         <v>Tempo em Hora</v>
       </c>
-      <c r="F13" s="8" t="str">
+      <c r="F12" s="15" t="str">
         <f>Sheet1!E11</f>
         <v>Custo Por Hora</v>
       </c>
-      <c r="G13" s="8" t="str">
+      <c r="G12" s="15" t="str">
         <f>Sheet1!F11</f>
         <v>Quantidade</v>
       </c>
-      <c r="H13" s="8" t="str">
+      <c r="H12" s="15" t="str">
         <f>Sheet1!G11</f>
         <v>Custo Total</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="8">
+    <row r="13" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="15">
         <f>Sheet1!B12</f>
         <v>1</v>
       </c>
-      <c r="D14" s="8" t="str">
+      <c r="D13" s="15" t="str">
         <f>Sheet1!C12</f>
         <v>Analista do Sistema</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E13" s="15">
         <f>Sheet1!D12</f>
         <v>10</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F13" s="15">
         <f>Sheet1!E12</f>
         <v>300</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G13" s="15">
         <f>Sheet1!F12</f>
         <v>1</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H13" s="15">
         <f>Sheet1!G12</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="8">
+    <row r="14" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="15">
         <f>Sheet1!B13</f>
         <v>2</v>
       </c>
-      <c r="D15" s="8" t="str">
+      <c r="D14" s="15" t="str">
         <f>Sheet1!C13</f>
         <v>Gestor de Proecto</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E14" s="15">
         <f>Sheet1!D13</f>
         <v>20</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F14" s="15">
         <f>Sheet1!E13</f>
         <v>500</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G14" s="15">
         <f>Sheet1!F13</f>
         <v>1</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H14" s="15">
         <f>Sheet1!G13</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="8">
+    <row r="15" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="15">
         <f>Sheet1!B14</f>
         <v>3</v>
       </c>
-      <c r="D16" s="8" t="str">
+      <c r="D15" s="15" t="str">
         <f>Sheet1!C14</f>
         <v>Eng Software Senior</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E15" s="15">
         <f>Sheet1!D14</f>
         <v>10</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F15" s="15">
         <f>Sheet1!E14</f>
         <v>400</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G15" s="15">
         <f>Sheet1!F14</f>
         <v>1</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H15" s="15">
         <f>Sheet1!G14</f>
         <v>4000</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="8">
+    <row r="16" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="15">
         <f>Sheet1!B15</f>
         <v>4</v>
       </c>
-      <c r="D17" s="8" t="str">
+      <c r="D16" s="15" t="str">
         <f>Sheet1!C15</f>
         <v>Eng Software Junior</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E16" s="15">
         <f>Sheet1!D15</f>
         <v>20</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F16" s="15">
         <f>Sheet1!E15</f>
         <v>250</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G16" s="15">
         <f>Sheet1!F15</f>
         <v>2</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H16" s="15">
         <f>Sheet1!G15</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="8" t="str">
+    <row r="17" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="15" t="str">
         <f>Sheet1!B16</f>
         <v>Total</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D17" s="15">
         <f>Sheet1!C16</f>
         <v>0</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E17" s="15">
         <f>Sheet1!D16</f>
         <v>60</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F17" s="15">
         <f>Sheet1!E16</f>
         <v>1450</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G17" s="15">
         <f>Sheet1!F16</f>
         <v>5</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H17" s="15">
         <f>Sheet1!G16</f>
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="12" t="str">
+    <row r="19" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="14" t="str">
         <f>Sheet1!B19</f>
         <v>Grupo de processo de Execução</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="8" t="s">
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="8" t="str">
+      <c r="D21" s="15" t="str">
         <f>Sheet1!C20</f>
         <v xml:space="preserve">Modulos </v>
       </c>
-      <c r="E22" s="8" t="str">
+      <c r="E21" s="15" t="str">
         <f>Sheet1!D20</f>
         <v>Designacao do Especialista</v>
       </c>
-      <c r="F22" s="8" t="str">
+      <c r="F21" s="15" t="str">
         <f>Sheet1!E20</f>
         <v>Tempo em Hora</v>
       </c>
-      <c r="G22" s="8" t="str">
+      <c r="G21" s="15" t="str">
         <f>Sheet1!F20</f>
         <v>Custo Por Hora</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I21" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="8">
-        <v>1</v>
-      </c>
-      <c r="D23" s="14" t="s">
+    <row r="22" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="15">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F22" s="15">
         <v>30</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G22" s="15">
         <v>200</v>
       </c>
-      <c r="H23" s="8">
-        <v>5</v>
-      </c>
-      <c r="I23" s="8">
-        <f>H23*G23*F23</f>
+      <c r="H22" s="15">
+        <v>5</v>
+      </c>
+      <c r="I22" s="15">
+        <f>H22*G22*F22</f>
         <v>30000</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="8">
+    <row r="23" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="15">
         <v>2</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="8" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F23" s="15">
         <v>10</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G23" s="15">
         <v>300</v>
       </c>
-      <c r="H24" s="8">
-        <v>1</v>
-      </c>
-      <c r="I24" s="8">
-        <f t="shared" ref="I24:I47" si="0">H24*G24*F24</f>
+      <c r="H23" s="15">
+        <v>1</v>
+      </c>
+      <c r="I23" s="15">
+        <f t="shared" ref="I23:I46" si="0">H23*G23*F23</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="8">
+    <row r="24" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="15">
         <v>3</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="8" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="8">
-        <v>5</v>
-      </c>
-      <c r="G25" s="8">
+      <c r="F24" s="15">
+        <v>5</v>
+      </c>
+      <c r="G24" s="15">
         <v>400</v>
       </c>
-      <c r="H25" s="8">
-        <v>1</v>
-      </c>
-      <c r="I25" s="8">
+      <c r="H24" s="15">
+        <v>1</v>
+      </c>
+      <c r="I24" s="15">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="8">
+    <row r="25" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="15">
         <v>4</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="8" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F25" s="15">
         <v>15</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G25" s="15">
         <v>250</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H25" s="15">
         <v>2</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I25" s="15">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="8">
-        <v>5</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="8" t="s">
+    <row r="26" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="15">
+        <v>5</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F26" s="15">
         <v>20</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G26" s="15">
         <v>500</v>
       </c>
-      <c r="H27" s="8">
-        <v>1</v>
-      </c>
-      <c r="I27" s="8">
+      <c r="H26" s="15">
+        <v>1</v>
+      </c>
+      <c r="I26" s="15">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="8">
+    <row r="27" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="15">
         <v>6</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D27" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E27" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F27" s="15">
         <v>30</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G27" s="15">
         <v>200</v>
       </c>
-      <c r="H28" s="8">
-        <v>5</v>
-      </c>
-      <c r="I28" s="8">
+      <c r="H27" s="15">
+        <v>5</v>
+      </c>
+      <c r="I27" s="15">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="8">
+    <row r="28" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="15">
         <v>7</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="8" t="s">
+      <c r="D28" s="16"/>
+      <c r="E28" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F28" s="15">
         <v>10</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G28" s="15">
         <v>300</v>
       </c>
-      <c r="H29" s="8">
-        <v>1</v>
-      </c>
-      <c r="I29" s="8">
+      <c r="H28" s="15">
+        <v>1</v>
+      </c>
+      <c r="I28" s="15">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="8">
+    <row r="29" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="15">
         <v>8</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="8" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="8">
-        <v>5</v>
-      </c>
-      <c r="G30" s="8">
+      <c r="F29" s="15">
+        <v>5</v>
+      </c>
+      <c r="G29" s="15">
         <v>400</v>
       </c>
-      <c r="H30" s="8">
-        <v>1</v>
-      </c>
-      <c r="I30" s="8">
+      <c r="H29" s="15">
+        <v>1</v>
+      </c>
+      <c r="I29" s="15">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="8">
+    <row r="30" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="15">
         <v>9</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="8" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F30" s="15">
         <v>15</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G30" s="15">
         <v>250</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H30" s="15">
         <v>2</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I30" s="15">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="8">
+    <row r="31" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="15">
         <v>10</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="8" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F31" s="15">
         <v>20</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G31" s="15">
         <v>500</v>
       </c>
-      <c r="H32" s="8">
-        <v>1</v>
-      </c>
-      <c r="I32" s="8">
+      <c r="H31" s="15">
+        <v>1</v>
+      </c>
+      <c r="I31" s="15">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="8">
+    <row r="32" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="15">
         <v>11</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D32" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E32" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F32" s="15">
         <v>30</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G32" s="15">
         <v>200</v>
       </c>
-      <c r="H33" s="8">
-        <v>5</v>
-      </c>
-      <c r="I33" s="8">
+      <c r="H32" s="15">
+        <v>5</v>
+      </c>
+      <c r="I32" s="15">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="8">
+    <row r="33" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="15">
         <v>12</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="8" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F33" s="15">
         <v>10</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G33" s="15">
         <v>300</v>
       </c>
-      <c r="H34" s="8">
-        <v>1</v>
-      </c>
-      <c r="I34" s="8">
+      <c r="H33" s="15">
+        <v>1</v>
+      </c>
+      <c r="I33" s="15">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="8">
+    <row r="34" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="15">
         <v>13</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="8" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F35" s="8">
-        <v>5</v>
-      </c>
-      <c r="G35" s="8">
+      <c r="F34" s="15">
+        <v>5</v>
+      </c>
+      <c r="G34" s="15">
         <v>400</v>
       </c>
-      <c r="H35" s="8">
-        <v>1</v>
-      </c>
-      <c r="I35" s="8">
+      <c r="H34" s="15">
+        <v>1</v>
+      </c>
+      <c r="I34" s="15">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C36" s="8">
+    <row r="35" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="15">
         <v>14</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="8" t="s">
+      <c r="D35" s="16"/>
+      <c r="E35" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F35" s="15">
         <v>15</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G35" s="15">
         <v>250</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H35" s="15">
         <v>2</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I35" s="15">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="8">
+    <row r="36" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="15">
         <v>15</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="8" t="s">
+      <c r="D36" s="16"/>
+      <c r="E36" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F36" s="15">
         <v>20</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G36" s="15">
         <v>500</v>
       </c>
-      <c r="H37" s="8">
-        <v>1</v>
-      </c>
-      <c r="I37" s="8">
+      <c r="H36" s="15">
+        <v>1</v>
+      </c>
+      <c r="I36" s="15">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="8">
+    <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="15">
         <v>16</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D37" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E37" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F37" s="15">
         <v>30</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G37" s="15">
         <v>200</v>
       </c>
-      <c r="H38" s="8">
-        <v>5</v>
-      </c>
-      <c r="I38" s="8">
+      <c r="H37" s="15">
+        <v>5</v>
+      </c>
+      <c r="I37" s="15">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="8">
+    <row r="38" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="15">
         <v>17</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="8" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F38" s="15">
         <v>10</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G38" s="15">
         <v>300</v>
       </c>
-      <c r="H39" s="8">
-        <v>1</v>
-      </c>
-      <c r="I39" s="8">
+      <c r="H38" s="15">
+        <v>1</v>
+      </c>
+      <c r="I38" s="15">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="8">
+    <row r="39" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="15">
         <v>18</v>
       </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="8" t="s">
+      <c r="D39" s="16"/>
+      <c r="E39" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F40" s="8">
-        <v>5</v>
-      </c>
-      <c r="G40" s="8">
+      <c r="F39" s="15">
+        <v>5</v>
+      </c>
+      <c r="G39" s="15">
         <v>400</v>
       </c>
-      <c r="H40" s="8">
-        <v>1</v>
-      </c>
-      <c r="I40" s="8">
+      <c r="H39" s="15">
+        <v>1</v>
+      </c>
+      <c r="I39" s="15">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="8">
+    <row r="40" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="15">
         <v>19</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="8" t="s">
+      <c r="D40" s="16"/>
+      <c r="E40" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F40" s="15">
         <v>15</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G40" s="15">
         <v>250</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H40" s="15">
         <v>2</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I40" s="15">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="8">
+    <row r="41" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="15">
         <v>20</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="8" t="s">
+      <c r="D41" s="16"/>
+      <c r="E41" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F41" s="15">
         <v>20</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G41" s="15">
         <v>500</v>
       </c>
-      <c r="H42" s="8">
-        <v>1</v>
-      </c>
-      <c r="I42" s="8">
+      <c r="H41" s="15">
+        <v>1</v>
+      </c>
+      <c r="I41" s="15">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C43" s="8">
+    <row r="42" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="15">
         <v>21</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D42" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E42" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F42" s="15">
         <v>30</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G42" s="15">
         <v>200</v>
       </c>
-      <c r="H43" s="8">
-        <v>5</v>
-      </c>
-      <c r="I43" s="8">
+      <c r="H42" s="15">
+        <v>5</v>
+      </c>
+      <c r="I42" s="15">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C44" s="8">
+    <row r="43" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="15">
         <v>22</v>
       </c>
-      <c r="D44" s="14"/>
-      <c r="E44" s="8" t="s">
+      <c r="D43" s="16"/>
+      <c r="E43" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F43" s="15">
         <v>10</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G43" s="15">
         <v>300</v>
       </c>
-      <c r="H44" s="8">
-        <v>1</v>
-      </c>
-      <c r="I44" s="8">
+      <c r="H43" s="15">
+        <v>1</v>
+      </c>
+      <c r="I43" s="15">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C45" s="8">
+    <row r="44" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="15">
         <v>23</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="8" t="s">
+      <c r="D44" s="16"/>
+      <c r="E44" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="8">
-        <v>5</v>
-      </c>
-      <c r="G45" s="8">
+      <c r="F44" s="15">
+        <v>5</v>
+      </c>
+      <c r="G44" s="15">
         <v>400</v>
       </c>
-      <c r="H45" s="8">
-        <v>1</v>
-      </c>
-      <c r="I45" s="8">
+      <c r="H44" s="15">
+        <v>1</v>
+      </c>
+      <c r="I44" s="15">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="8">
+    <row r="45" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="15">
         <v>24</v>
       </c>
-      <c r="D46" s="14"/>
-      <c r="E46" s="8" t="s">
+      <c r="D45" s="16"/>
+      <c r="E45" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F45" s="15">
         <v>15</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G45" s="15">
         <v>250</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H45" s="15">
         <v>2</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I45" s="15">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C47" s="8">
+    <row r="46" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="15">
         <v>25</v>
       </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="8" t="s">
+      <c r="D46" s="16"/>
+      <c r="E46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F46" s="15">
         <v>20</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G46" s="15">
         <v>500</v>
       </c>
-      <c r="H47" s="8">
-        <v>1</v>
-      </c>
-      <c r="I47" s="8">
+      <c r="H46" s="15">
+        <v>1</v>
+      </c>
+      <c r="I46" s="15">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="15"/>
+      <c r="D47" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15">
+        <f>SUM(F22:F46)</f>
+        <v>400</v>
+      </c>
+      <c r="G47" s="15">
+        <f t="shared" ref="G47:H47" si="1">SUM(G22:G46)</f>
+        <v>8250</v>
+      </c>
+      <c r="H47" s="15">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I47" s="17">
+        <f>SUM(I22:I46)</f>
+        <v>262500</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
-      <c r="I48" s="17">
-        <f>SUM(I23:I47)</f>
-        <v>262500</v>
-      </c>
-    </row>
-    <row r="49" spans="3:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="19"/>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="3:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="9"/>
     </row>
     <row r="50" spans="3:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="19"/>
-    </row>
-    <row r="51" spans="3:9" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="3:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="19"/>
-    </row>
-    <row r="52" spans="3:9" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="8" t="s">
+      <c r="D51" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F51" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G51" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H51" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I52" s="19"/>
-    </row>
-    <row r="53" spans="3:9" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="7">
-        <v>1</v>
-      </c>
-      <c r="D53" s="8" t="s">
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="3:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="15">
+        <v>1</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E52" s="15">
+        <v>5</v>
+      </c>
+      <c r="F52" s="15">
+        <v>400</v>
+      </c>
+      <c r="G52" s="15">
+        <v>1</v>
+      </c>
+      <c r="H52" s="15">
+        <f>E52*F52*G52</f>
+        <v>2000</v>
+      </c>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="3:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="15">
+        <v>2</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="15">
+        <v>5</v>
+      </c>
+      <c r="F53" s="15">
+        <v>250</v>
+      </c>
+      <c r="G53" s="15">
+        <v>1</v>
+      </c>
+      <c r="H53" s="15">
+        <f t="shared" ref="H53:H55" si="2">E53*F53*G53</f>
+        <v>1250</v>
+      </c>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="3:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="15">
         <v>3</v>
       </c>
-      <c r="F53" s="7">
-        <v>400</v>
-      </c>
-      <c r="G53" s="7">
-        <v>1</v>
-      </c>
-      <c r="H53" s="7">
-        <f>E53*F53*G53</f>
-        <v>1200</v>
-      </c>
-      <c r="I53" s="19"/>
-    </row>
-    <row r="54" spans="3:9" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="7">
-        <v>2</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E54" s="7">
-        <v>5</v>
-      </c>
-      <c r="F54" s="7">
-        <v>250</v>
-      </c>
-      <c r="G54" s="7">
-        <v>1</v>
-      </c>
-      <c r="H54" s="7">
-        <f t="shared" ref="H54:H56" si="1">E54*F54*G54</f>
-        <v>1250</v>
-      </c>
-      <c r="I54" s="19"/>
-    </row>
-    <row r="55" spans="3:9" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="7">
+      <c r="D54" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="15">
+        <v>5</v>
+      </c>
+      <c r="F54" s="15">
+        <v>500</v>
+      </c>
+      <c r="G54" s="15">
+        <v>1</v>
+      </c>
+      <c r="H54" s="15">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="3:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="15">
+        <v>4</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="15">
+        <f>E52+E54+E53</f>
+        <v>15</v>
+      </c>
+      <c r="F55" s="15">
+        <f>F52+F53+F54</f>
+        <v>1150</v>
+      </c>
+      <c r="G55" s="15">
         <v>3</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" s="7">
-        <v>5</v>
-      </c>
-      <c r="F55" s="7">
-        <v>500</v>
-      </c>
-      <c r="G55" s="7">
-        <v>1</v>
-      </c>
-      <c r="H55" s="7">
-        <f t="shared" si="1"/>
-        <v>2500</v>
-      </c>
-      <c r="I55" s="19"/>
-    </row>
-    <row r="56" spans="3:9" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="7">
-        <v>4</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="7">
-        <f>E53+E55+E54</f>
-        <v>13</v>
-      </c>
-      <c r="F56" s="7">
-        <f>F53+F54+F55</f>
-        <v>1150</v>
-      </c>
-      <c r="G56" s="7">
-        <v>3</v>
-      </c>
-      <c r="H56" s="7">
-        <f t="shared" si="1"/>
-        <v>44850</v>
-      </c>
-      <c r="I56" s="19"/>
-    </row>
-    <row r="57" spans="3:9" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="19"/>
+      <c r="H55" s="15">
+        <f t="shared" si="2"/>
+        <v>51750</v>
+      </c>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="3:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="D42:D46"/>
     <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="D28:D32"/>
-    <mergeCell ref="D33:D37"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="D32:D36"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>